<commit_message>
fixed bug in GF classes
</commit_message>
<xml_diff>
--- a/Data/E4.xlsx
+++ b/Data/E4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="2" r:id="rId1"/>
@@ -1699,7 +1699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -2107,8 +2107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>